<commit_message>
18/4/5 TVA.tex Exp-results=>Finish begining
</commit_message>
<xml_diff>
--- a/DATE2018/exp/maui_exp.xlsx
+++ b/DATE2018/exp/maui_exp.xlsx
@@ -1,25 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lishoujun/Desktop/Paper_Latex/maui/exp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erictseng 1/Desktop/LaTeX/MAUI-Latex/DATE2018/exp/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{23FCC190-0E67-214D-935C-E8E82B390267}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Benchmark info" sheetId="1" r:id="rId1"/>
-    <sheet name="Experimental Result (Non-CG)" sheetId="5" r:id="rId2"/>
-    <sheet name="Boundary vs Improvement" sheetId="6" r:id="rId3"/>
+    <sheet name="Benchmark info (2)" sheetId="7" r:id="rId1"/>
+    <sheet name="Benchmark info" sheetId="1" r:id="rId2"/>
+    <sheet name="Experimental Result (Non-CG)" sheetId="5" r:id="rId3"/>
+    <sheet name="Boundary vs Improvement" sheetId="6" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="57">
   <si>
     <t>(ps)</t>
   </si>
@@ -252,11 +251,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -344,7 +343,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="47">
     <border>
       <left/>
       <right/>
@@ -909,6 +908,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -927,7 +979,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1144,6 +1196,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="38" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="7" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1225,61 +1325,112 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="38" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="7" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="百分比" xfId="1" builtinId="5"/>
-    <cellStyle name="百分比 2" xfId="2"/>
-    <cellStyle name="百分比 3" xfId="3"/>
-    <cellStyle name="百分比 4" xfId="4"/>
+    <cellStyle name="百分比 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="百分比 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="百分比 4" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1287,12 +1438,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-TW"/>
   <c:roundedCorners val="0"/>
@@ -1342,7 +1496,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1381,8 +1534,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.108456535652049"/>
           <c:y val="0.118790151231096"/>
-          <c:w val="0.802237099774831"/>
-          <c:h val="0.737009437105805"/>
+          <c:w val="0.80223709977483104"/>
+          <c:h val="0.73700943710580502"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1425,28 +1578,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1458,34 +1611,34 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.152542372881356</c:v>
+                  <c:v>0.15254237288135578</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.152542372881356</c:v>
+                  <c:v>0.15254237288135578</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.182405165456012</c:v>
+                  <c:v>0.18240516545601221</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.386602098466505</c:v>
+                  <c:v>0.38660209846650512</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.48910411622276</c:v>
+                  <c:v>0.48910411622275962</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.48910411622276</c:v>
+                  <c:v>0.48910411622275962</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.48910411622276</c:v>
+                  <c:v>0.48910411622275962</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.48910411622276</c:v>
+                  <c:v>0.48910411622275962</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-357D-40A1-B6A7-C771E4437432}"/>
             </c:ext>
@@ -1545,28 +1698,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1578,34 +1731,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28.0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>28.0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28.0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>28.0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-357D-40A1-B6A7-C771E4437432}"/>
             </c:ext>
@@ -1663,8 +1816,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.00159445210411886"/>
-              <c:y val="0.315978616456044"/>
+              <c:x val="1.5944521041188599E-3"/>
+              <c:y val="0.31597861645604403"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1772,8 +1925,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.414904491358018"/>
-              <c:y val="0.930484410125715"/>
+              <c:x val="0.41490449135801799"/>
+              <c:y val="0.93048441012571503"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1853,7 +2006,7 @@
         <c:axId val="-2099036528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0.0"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -1888,8 +2041,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.963406198326779"/>
-              <c:y val="0.41628216120812"/>
+              <c:x val="0.96340619832677898"/>
+              <c:y val="0.41628216120812001"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1991,10 +2144,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.679558154474398"/>
-          <c:y val="0.732517704960822"/>
-          <c:w val="0.226527799072358"/>
-          <c:h val="0.115286247796161"/>
+          <c:x val="0.67955815447439805"/>
+          <c:y val="0.73251770496082202"/>
+          <c:w val="0.22652779907235801"/>
+          <c:h val="0.11528624779616101"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2625,20 +2778,26 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>94195</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>202138</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="753155" cy="266355"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="2" name="文字方塊 1"/>
+            <xdr:cNvPr id="2" name="文字方塊 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B8D4104-CD66-9B42-ACF3-F07B52B613AA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvSpPr txBox="1"/>
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6888695" y="684738"/>
+              <a:off x="7002995" y="684738"/>
               <a:ext cx="753155" cy="266355"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2677,7 +2836,7 @@
                       <m:sSubPr>
                         <m:ctrlPr>
                           <a:rPr lang="en-US" altLang="zh-TW" sz="1600" i="1">
-                            <a:latin typeface="Cambria Math" charset="0"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
                       </m:sSubPr>
@@ -2751,10 +2910,1010 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="2" name="文字方塊 1"/>
+            <xdr:cNvPr id="2" name="文字方塊 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B8D4104-CD66-9B42-ACF3-F07B52B613AA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7002995" y="684738"/>
+              <a:ext cx="753155" cy="266355"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="zh-TW" altLang="en-US" sz="1600" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑇</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-TW" sz="1600" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>_(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-TW" altLang="en-US" sz="1600" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑐</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-TW" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>_𝑓𝑟𝑒𝑠ℎ</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-TW" altLang="en-US" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>"</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-TW" altLang="en-US" sz="1600" i="0">
+                  <a:effectLst/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-TW" altLang="en-US" sz="1600" i="0">
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>" </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-TW" sz="1600" i="0">
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>)</a:t>
+              </a:r>
+              <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1200"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>59273</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>219072</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="706604" cy="266611"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="文字方塊 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F47DE21-A957-6F4D-9072-72CB6248BF0E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7882473" y="701672"/>
+              <a:ext cx="706604" cy="266611"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" altLang="zh-TW" sz="1600" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="zh-TW" altLang="en-US" sz="1600" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑇</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="zh-TW" altLang="en-US" sz="1600" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑐</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-TW" sz="1600" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>_</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-TW" sz="1600" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑎𝑔𝑒𝑑</m:t>
+                        </m:r>
+                        <m:r>
+                          <m:rPr>
+                            <m:nor/>
+                          </m:rPr>
+                          <a:rPr lang="zh-TW" altLang="en-US" sz="1600">
+                            <a:effectLst/>
+                          </a:rPr>
+                          <m:t> </m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1600"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="文字方塊 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F47DE21-A957-6F4D-9072-72CB6248BF0E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7882473" y="701672"/>
+              <a:ext cx="706604" cy="266611"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="zh-TW" altLang="en-US" sz="1600" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑇</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-TW" sz="1600" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>_(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-TW" altLang="en-US" sz="1600" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑐</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-TW" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>_𝑎𝑔𝑒𝑑</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-TW" altLang="en-US" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>"</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-TW" altLang="en-US" sz="1600" i="0">
+                  <a:effectLst/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-TW" altLang="en-US" sz="1600" i="0">
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>" </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-TW" sz="1600" i="0">
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>)</a:t>
+              </a:r>
+              <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1600"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>59268</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>203198</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1015343" cy="266611"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="文字方塊 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2144D73-2863-AD45-95CD-596981E153B9}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8644468" y="685798"/>
+              <a:ext cx="1015343" cy="266611"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" altLang="zh-TW" sz="1600" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="zh-TW" altLang="en-US" sz="1600" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑇</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="zh-TW" altLang="en-US" sz="1600" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑐</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-TW" sz="1600" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>_</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-TW" sz="1600" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑎𝑔𝑒𝑑</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-TW" sz="1600" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>_</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-TW" sz="1600" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑜𝑝𝑡</m:t>
+                        </m:r>
+                        <m:r>
+                          <m:rPr>
+                            <m:nor/>
+                          </m:rPr>
+                          <a:rPr lang="zh-TW" altLang="en-US" sz="1600">
+                            <a:effectLst/>
+                          </a:rPr>
+                          <m:t> </m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1600"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="文字方塊 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2144D73-2863-AD45-95CD-596981E153B9}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8644468" y="685798"/>
+              <a:ext cx="1015343" cy="266611"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="zh-TW" altLang="en-US" sz="1600" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑇</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-TW" sz="1600" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>_(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-TW" altLang="en-US" sz="1600" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑐</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-TW" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>_𝑎𝑔𝑒𝑑_𝑜𝑝𝑡</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-TW" altLang="en-US" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>"</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-TW" altLang="en-US" sz="1600" i="0">
+                  <a:effectLst/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-TW" altLang="en-US" sz="1600" i="0">
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>" </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-TW" sz="1600" i="0">
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>)</a:t>
+              </a:r>
+              <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1600"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>59268</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>203198</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1015343" cy="266611"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="文字方塊 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BC0C70C-A2D1-6148-8D08-88C838FEDFB3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9406468" y="685798"/>
+              <a:ext cx="1015343" cy="266611"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" altLang="zh-TW" sz="1600" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="zh-TW" altLang="en-US" sz="1600" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑇</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="zh-TW" altLang="en-US" sz="1600" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑐</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-TW" sz="1600" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>_</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-TW" sz="1600" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑎𝑔𝑒𝑑</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-TW" sz="1600" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>_</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-TW" sz="1600" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑜𝑝𝑡</m:t>
+                        </m:r>
+                        <m:r>
+                          <m:rPr>
+                            <m:nor/>
+                          </m:rPr>
+                          <a:rPr lang="zh-TW" altLang="en-US" sz="1600">
+                            <a:effectLst/>
+                          </a:rPr>
+                          <m:t> </m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1600"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="文字方塊 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BC0C70C-A2D1-6148-8D08-88C838FEDFB3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9406468" y="685798"/>
+              <a:ext cx="1015343" cy="266611"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="zh-TW" altLang="en-US" sz="1600" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑇</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-TW" sz="1600" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>_(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-TW" altLang="en-US" sz="1600" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑐</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-TW" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>_𝑎𝑔𝑒𝑑_𝑜𝑝𝑡</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-TW" altLang="en-US" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>"</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-TW" altLang="en-US" sz="1600" i="0">
+                  <a:effectLst/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="zh-TW" altLang="en-US" sz="1600" i="0">
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>" </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="zh-TW" sz="1600" i="0">
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>)</a:t>
+              </a:r>
+              <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1600"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>94195</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>202138</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="753155" cy="266355"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="文字方塊 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvSpPr txBox="1"/>
           </xdr:nvSpPr>
           <xdr:spPr>
@@ -2788,6 +3947,135 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" altLang="zh-TW" sz="1600" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="zh-TW" altLang="en-US" sz="1600" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑇</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="zh-TW" altLang="en-US" sz="1600" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑐</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-TW" sz="1600" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>_</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" altLang="zh-TW" sz="1600" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑓𝑟𝑒𝑠h</m:t>
+                        </m:r>
+                        <m:r>
+                          <m:rPr>
+                            <m:nor/>
+                          </m:rPr>
+                          <a:rPr lang="zh-TW" altLang="en-US" sz="1600">
+                            <a:effectLst/>
+                            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t> </m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1200"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="文字方塊 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6888695" y="684738"/>
+              <a:ext cx="753155" cy="266355"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="zh-TW" altLang="en-US" sz="1600" i="0">
                   <a:solidFill>
@@ -2806,7 +4094,7 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="Cambria Math" charset="0"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
@@ -2851,20 +4139,24 @@
               <a:r>
                 <a:rPr lang="zh-TW" altLang="en-US" sz="1600" i="0">
                   <a:effectLst/>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:rPr>
                 <a:t> </a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="zh-TW" altLang="en-US" sz="1600" i="0">
                   <a:effectLst/>
-                  <a:latin typeface="Cambria Math" charset="0"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:rPr>
                 <a:t>" </a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" altLang="zh-TW" sz="1600" i="0">
                   <a:effectLst/>
-                  <a:latin typeface="Cambria Math" charset="0"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:rPr>
                 <a:t>)</a:t>
               </a:r>
@@ -2888,7 +4180,13 @@
       <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="3" name="文字方塊 2"/>
+            <xdr:cNvPr id="3" name="文字方塊 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvSpPr txBox="1"/>
           </xdr:nvSpPr>
           <xdr:spPr>
@@ -2932,7 +4230,7 @@
                       <m:sSubPr>
                         <m:ctrlPr>
                           <a:rPr lang="en-US" altLang="zh-TW" sz="1600" i="1">
-                            <a:latin typeface="Cambria Math" charset="0"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
                       </m:sSubPr>
@@ -3143,7 +4441,13 @@
       <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="4" name="文字方塊 3"/>
+            <xdr:cNvPr id="4" name="文字方塊 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvSpPr txBox="1"/>
           </xdr:nvSpPr>
           <xdr:spPr>
@@ -3187,7 +4491,7 @@
                       <m:sSubPr>
                         <m:ctrlPr>
                           <a:rPr lang="en-US" altLang="zh-TW" sz="1600" i="1">
-                            <a:latin typeface="Cambria Math" charset="0"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
                       </m:sSubPr>
@@ -3413,7 +4717,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -3427,7 +4731,13 @@
       <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="2" name="文字方塊 1"/>
+            <xdr:cNvPr id="2" name="文字方塊 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvSpPr txBox="1"/>
           </xdr:nvSpPr>
           <xdr:spPr>
@@ -3471,7 +4781,7 @@
                       <m:sSubPr>
                         <m:ctrlPr>
                           <a:rPr lang="en-US" altLang="zh-TW" sz="1600" i="1">
-                            <a:latin typeface="Cambria Math" charset="0"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
                       </m:sSubPr>
@@ -3682,7 +4992,13 @@
       <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="3" name="文字方塊 2"/>
+            <xdr:cNvPr id="3" name="文字方塊 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvSpPr txBox="1"/>
           </xdr:nvSpPr>
           <xdr:spPr>
@@ -3726,7 +5042,7 @@
                       <m:sSubPr>
                         <m:ctrlPr>
                           <a:rPr lang="en-US" altLang="zh-TW" sz="1600" i="1">
-                            <a:latin typeface="Cambria Math" charset="0"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
                       </m:sSubPr>
@@ -3937,7 +5253,13 @@
       <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="4" name="文字方塊 3"/>
+            <xdr:cNvPr id="4" name="文字方塊 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvSpPr txBox="1"/>
           </xdr:nvSpPr>
           <xdr:spPr>
@@ -3981,7 +5303,7 @@
                       <m:sSubPr>
                         <m:ctrlPr>
                           <a:rPr lang="en-US" altLang="zh-TW" sz="1600" i="1">
-                            <a:latin typeface="Cambria Math" charset="0"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
                       </m:sSubPr>
@@ -4207,7 +5529,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4224,7 +5546,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="圖表 1"/>
+        <xdr:cNvPr id="2" name="圖表 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -4242,120 +5570,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Notations"/>
-      <sheetName val="Benchmark info"/>
-      <sheetName val="Experimental Result (Non-CG)"/>
-      <sheetName val="Experimental Result (CG)"/>
-      <sheetName val="Runtime"/>
-      <sheetName val="Boundary vs Improvement"/>
-      <sheetName val="Aging impaected on DCCs"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5">
-        <row r="3">
-          <cell r="B3">
-            <v>2</v>
-          </cell>
-          <cell r="F3">
-            <v>0.15254237288135578</v>
-          </cell>
-          <cell r="G3">
-            <v>4</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4">
-            <v>3</v>
-          </cell>
-          <cell r="F4">
-            <v>0.15254237288135578</v>
-          </cell>
-          <cell r="G4">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5">
-            <v>4</v>
-          </cell>
-          <cell r="F5">
-            <v>0.18240516545601221</v>
-          </cell>
-          <cell r="G5">
-            <v>7</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6">
-            <v>5</v>
-          </cell>
-          <cell r="F6">
-            <v>0.38660209846650512</v>
-          </cell>
-          <cell r="G6">
-            <v>16</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7">
-            <v>6</v>
-          </cell>
-          <cell r="F7">
-            <v>0.48910411622275962</v>
-          </cell>
-          <cell r="G7">
-            <v>28</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8">
-            <v>7</v>
-          </cell>
-          <cell r="F8">
-            <v>0.48910411622275962</v>
-          </cell>
-          <cell r="G8">
-            <v>28</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9">
-            <v>8</v>
-          </cell>
-          <cell r="F9">
-            <v>0.48910411622275962</v>
-          </cell>
-          <cell r="G9">
-            <v>28</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10">
-            <v>9</v>
-          </cell>
-          <cell r="F10">
-            <v>0.48910411622275962</v>
-          </cell>
-          <cell r="G10">
-            <v>28</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="6"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4620,14 +5834,505 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23DC462A-3CD6-5D40-9A48-8A31CE3AE51B}">
+  <dimension ref="B1:M15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="10" max="11" width="14" customWidth="1"/>
+    <col min="12" max="12" width="11.1640625" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" customWidth="1"/>
+    <col min="17" max="17" width="10" customWidth="1"/>
+    <col min="18" max="18" width="18.1640625" customWidth="1"/>
+    <col min="19" max="19" width="18.6640625" customWidth="1"/>
+    <col min="20" max="20" width="12.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:13" ht="16" thickBot="1"/>
+    <row r="2" spans="2:13" ht="22.75" customHeight="1" thickTop="1">
+      <c r="B2" s="92" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="90" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="90" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="94" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="94" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="96" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="98" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="100" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="88" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" ht="22.75" customHeight="1">
+      <c r="B3" s="115"/>
+      <c r="C3" s="116"/>
+      <c r="D3" s="116"/>
+      <c r="E3" s="117"/>
+      <c r="F3" s="117"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="119"/>
+      <c r="I3" s="120"/>
+      <c r="J3" s="121"/>
+      <c r="K3" s="121"/>
+      <c r="L3" s="122"/>
+      <c r="M3" s="122"/>
+    </row>
+    <row r="4" spans="2:13" ht="56" customHeight="1" thickBot="1">
+      <c r="B4" s="93"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="95"/>
+      <c r="F4" s="95"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="101"/>
+      <c r="M4" s="89"/>
+    </row>
+    <row r="5" spans="2:13" ht="22" thickTop="1">
+      <c r="B5" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="24">
+        <v>7401</v>
+      </c>
+      <c r="D5" s="24">
+        <v>8802</v>
+      </c>
+      <c r="E5" s="23">
+        <v>3416</v>
+      </c>
+      <c r="F5" s="23">
+        <v>3416</v>
+      </c>
+      <c r="G5" s="22">
+        <v>11</v>
+      </c>
+      <c r="H5" s="29">
+        <v>773.9</v>
+      </c>
+      <c r="I5" s="28">
+        <v>897.8</v>
+      </c>
+      <c r="J5" s="27">
+        <v>849.9</v>
+      </c>
+      <c r="K5" s="27">
+        <v>849.9</v>
+      </c>
+      <c r="L5" s="26">
+        <f t="shared" ref="L5:L13" si="0">(I5-K5)/(I5-H5)*100%</f>
+        <v>0.38660209846650512</v>
+      </c>
+      <c r="M5" s="25">
+        <v>16.45</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" ht="21">
+      <c r="B6" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="16">
+        <v>526297</v>
+      </c>
+      <c r="D6" s="16">
+        <v>108839</v>
+      </c>
+      <c r="E6" s="15">
+        <v>26863</v>
+      </c>
+      <c r="F6" s="15">
+        <v>4924</v>
+      </c>
+      <c r="G6" s="14">
+        <v>10</v>
+      </c>
+      <c r="H6" s="21">
+        <v>3016.7</v>
+      </c>
+      <c r="I6" s="20">
+        <v>3530.6</v>
+      </c>
+      <c r="J6" s="19">
+        <v>3458.5</v>
+      </c>
+      <c r="K6" s="19">
+        <v>3458.5</v>
+      </c>
+      <c r="L6" s="18">
+        <f t="shared" si="0"/>
+        <v>0.14029966919634149</v>
+      </c>
+      <c r="M6" s="17">
+        <v>24.89</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" ht="21">
+      <c r="B7" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="16">
+        <v>561091</v>
+      </c>
+      <c r="D7" s="16">
+        <v>97831</v>
+      </c>
+      <c r="E7" s="15">
+        <v>33651</v>
+      </c>
+      <c r="F7" s="15">
+        <v>7904</v>
+      </c>
+      <c r="G7" s="14">
+        <v>12</v>
+      </c>
+      <c r="H7" s="21">
+        <v>3367</v>
+      </c>
+      <c r="I7" s="20">
+        <v>3940.2</v>
+      </c>
+      <c r="J7" s="19">
+        <v>3897.9</v>
+      </c>
+      <c r="K7" s="19">
+        <v>3897.9</v>
+      </c>
+      <c r="L7" s="18">
+        <f t="shared" si="0"/>
+        <v>7.3796231681786006E-2</v>
+      </c>
+      <c r="M7" s="17">
+        <v>30.69</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" ht="21">
+      <c r="B8" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="16">
+        <v>101496</v>
+      </c>
+      <c r="D8" s="16">
+        <v>17079</v>
+      </c>
+      <c r="E8" s="15">
+        <v>5030</v>
+      </c>
+      <c r="F8" s="15">
+        <v>4345</v>
+      </c>
+      <c r="G8" s="14">
+        <v>10</v>
+      </c>
+      <c r="H8" s="21">
+        <v>864.2</v>
+      </c>
+      <c r="I8" s="20">
+        <v>1013.7</v>
+      </c>
+      <c r="J8" s="19">
+        <v>994.1</v>
+      </c>
+      <c r="K8" s="19">
+        <v>994.1</v>
+      </c>
+      <c r="L8" s="18">
+        <f t="shared" si="0"/>
+        <v>0.13110367892976604</v>
+      </c>
+      <c r="M8" s="17">
+        <v>32.770000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="21">
+      <c r="B9" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="16">
+        <v>2627</v>
+      </c>
+      <c r="D9" s="16">
+        <v>625</v>
+      </c>
+      <c r="E9" s="15">
+        <v>186</v>
+      </c>
+      <c r="F9" s="15">
+        <v>180</v>
+      </c>
+      <c r="G9" s="14">
+        <v>8</v>
+      </c>
+      <c r="H9" s="21">
+        <v>776.3</v>
+      </c>
+      <c r="I9" s="20">
+        <v>891.7</v>
+      </c>
+      <c r="J9" s="19">
+        <v>873.3</v>
+      </c>
+      <c r="K9" s="19">
+        <v>873.3</v>
+      </c>
+      <c r="L9" s="18">
+        <f t="shared" si="0"/>
+        <v>0.15944540727903012</v>
+      </c>
+      <c r="M9" s="17">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" ht="21">
+      <c r="B10" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="16">
+        <v>2967</v>
+      </c>
+      <c r="D10" s="16">
+        <v>513</v>
+      </c>
+      <c r="E10" s="15">
+        <v>100</v>
+      </c>
+      <c r="F10" s="15">
+        <v>100</v>
+      </c>
+      <c r="G10" s="14">
+        <v>5</v>
+      </c>
+      <c r="H10" s="21">
+        <v>1011.1</v>
+      </c>
+      <c r="I10" s="20">
+        <v>1165.9000000000001</v>
+      </c>
+      <c r="J10" s="19">
+        <v>1089.9000000000001</v>
+      </c>
+      <c r="K10" s="19">
+        <v>1089.9000000000001</v>
+      </c>
+      <c r="L10" s="18">
+        <f t="shared" si="0"/>
+        <v>0.49095607235142097</v>
+      </c>
+      <c r="M10" s="17">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" ht="21">
+      <c r="B11" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="16">
+        <v>6466</v>
+      </c>
+      <c r="D11" s="16">
+        <v>1728</v>
+      </c>
+      <c r="E11" s="15">
+        <v>411</v>
+      </c>
+      <c r="F11" s="15">
+        <v>411</v>
+      </c>
+      <c r="G11" s="14">
+        <v>6</v>
+      </c>
+      <c r="H11" s="21">
+        <v>822.1</v>
+      </c>
+      <c r="I11" s="20">
+        <v>950.8</v>
+      </c>
+      <c r="J11" s="19">
+        <v>886.6</v>
+      </c>
+      <c r="K11" s="19">
+        <v>886.6</v>
+      </c>
+      <c r="L11" s="18">
+        <f t="shared" si="0"/>
+        <v>0.4988344988344986</v>
+      </c>
+      <c r="M11" s="17">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" ht="21">
+      <c r="B12" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="16">
+        <v>8422</v>
+      </c>
+      <c r="D12" s="16">
+        <v>1564</v>
+      </c>
+      <c r="E12" s="15">
+        <v>376</v>
+      </c>
+      <c r="F12" s="15">
+        <v>376</v>
+      </c>
+      <c r="G12" s="14">
+        <v>6</v>
+      </c>
+      <c r="H12" s="21">
+        <v>798.1</v>
+      </c>
+      <c r="I12" s="20">
+        <v>933.2</v>
+      </c>
+      <c r="J12" s="19">
+        <v>909.8</v>
+      </c>
+      <c r="K12" s="19">
+        <v>909.8</v>
+      </c>
+      <c r="L12" s="18">
+        <f t="shared" si="0"/>
+        <v>0.17320503330866088</v>
+      </c>
+      <c r="M12" s="17">
+        <v>1.46</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" ht="22" thickBot="1">
+      <c r="B13" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="13">
+        <v>6861</v>
+      </c>
+      <c r="D13" s="13">
+        <v>1275</v>
+      </c>
+      <c r="E13" s="12">
+        <v>627</v>
+      </c>
+      <c r="F13" s="12">
+        <v>557</v>
+      </c>
+      <c r="G13" s="11">
+        <v>10</v>
+      </c>
+      <c r="H13" s="10">
+        <v>731.7</v>
+      </c>
+      <c r="I13" s="9">
+        <v>842.5</v>
+      </c>
+      <c r="J13" s="8">
+        <v>820.3</v>
+      </c>
+      <c r="K13" s="8">
+        <v>820.3</v>
+      </c>
+      <c r="L13" s="7">
+        <f t="shared" si="0"/>
+        <v>0.2003610108303254</v>
+      </c>
+      <c r="M13" s="6">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" ht="23" thickTop="1" thickBot="1">
+      <c r="B14" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1">
+        <f>AVERAGE(L5:L13)</f>
+        <v>0.25051152231981499</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" ht="16" thickTop="1"/>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+  </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="5" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
@@ -4647,378 +6352,378 @@
     <col min="19" max="19" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:12" ht="22.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="76" t="s">
+    <row r="1" spans="2:12" ht="16" thickBot="1"/>
+    <row r="2" spans="2:12" ht="22.75" customHeight="1" thickTop="1">
+      <c r="B2" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="74" t="s">
+      <c r="C2" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="74" t="s">
+      <c r="D2" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="78" t="s">
+      <c r="E2" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="78" t="s">
+      <c r="F2" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="80" t="s">
+      <c r="G2" s="96" t="s">
         <v>12</v>
       </c>
       <c r="H2" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="82" t="s">
+      <c r="I2" s="98" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="83"/>
-      <c r="K2" s="84" t="s">
+      <c r="J2" s="99"/>
+      <c r="K2" s="100" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="72" t="s">
+      <c r="L2" s="88" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="77"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="81"/>
+    <row r="3" spans="2:12" ht="56" customHeight="1" thickBot="1">
+      <c r="B3" s="93"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="97"/>
       <c r="H3" s="35"/>
       <c r="I3" s="36"/>
       <c r="J3" s="37"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="73"/>
+      <c r="K3" s="101"/>
+      <c r="L3" s="89"/>
     </row>
-    <row r="4" spans="2:12" ht="22" thickTop="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:12" ht="21" thickTop="1">
       <c r="B4" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="123">
         <v>7401</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="123">
         <v>8802</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="124">
         <v>3416</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="124">
         <v>3416</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="125">
         <v>11</v>
       </c>
-      <c r="H4" s="29">
+      <c r="H4" s="126">
         <v>773.9</v>
       </c>
-      <c r="I4" s="28">
+      <c r="I4" s="127">
         <v>897.8</v>
       </c>
-      <c r="J4" s="27">
+      <c r="J4" s="128">
         <v>849.9</v>
       </c>
-      <c r="K4" s="26">
+      <c r="K4" s="129">
         <f t="shared" ref="K4:K12" si="0">(I4-J4)/(I4-H4)*100%</f>
         <v>0.38660209846650512</v>
       </c>
-      <c r="L4" s="25">
+      <c r="L4" s="130">
         <v>16.45</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="21" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:12" ht="20">
       <c r="B5" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="131">
         <v>526297</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="131">
         <v>108839</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="132">
         <v>26863</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="132">
         <v>4924</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="133">
         <v>10</v>
       </c>
-      <c r="H5" s="21">
+      <c r="H5" s="134">
         <v>3016.7</v>
       </c>
-      <c r="I5" s="20">
+      <c r="I5" s="135">
         <v>3530.6</v>
       </c>
-      <c r="J5" s="19">
+      <c r="J5" s="136">
         <v>3458.5</v>
       </c>
-      <c r="K5" s="18">
+      <c r="K5" s="137">
         <f t="shared" si="0"/>
         <v>0.14029966919634149</v>
       </c>
-      <c r="L5" s="17">
+      <c r="L5" s="138">
         <v>24.89</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="21" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:12" ht="20">
       <c r="B6" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="131">
         <v>561091</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="131">
         <v>97831</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="132">
         <v>33651</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="132">
         <v>7904</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="133">
         <v>12</v>
       </c>
-      <c r="H6" s="21">
+      <c r="H6" s="134">
         <v>3367</v>
       </c>
-      <c r="I6" s="20">
+      <c r="I6" s="135">
         <v>3940.2</v>
       </c>
-      <c r="J6" s="19">
+      <c r="J6" s="136">
         <v>3897.9</v>
       </c>
-      <c r="K6" s="18">
+      <c r="K6" s="137">
         <f t="shared" si="0"/>
         <v>7.3796231681786006E-2</v>
       </c>
-      <c r="L6" s="17">
+      <c r="L6" s="138">
         <v>30.69</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="21" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:12" ht="20">
       <c r="B7" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="131">
         <v>101496</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="131">
         <v>17079</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="132">
         <v>5030</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="132">
         <v>4345</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="133">
         <v>10</v>
       </c>
-      <c r="H7" s="21">
+      <c r="H7" s="134">
         <v>864.2</v>
       </c>
-      <c r="I7" s="20">
+      <c r="I7" s="135">
         <v>1013.7</v>
       </c>
-      <c r="J7" s="19">
+      <c r="J7" s="136">
         <v>994.1</v>
       </c>
-      <c r="K7" s="18">
+      <c r="K7" s="137">
         <f t="shared" si="0"/>
         <v>0.13110367892976604</v>
       </c>
-      <c r="L7" s="17">
+      <c r="L7" s="138">
         <v>32.770000000000003</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="21" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:12" ht="20">
       <c r="B8" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="131">
         <v>2627</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="131">
         <v>625</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="132">
         <v>186</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="132">
         <v>180</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="133">
         <v>8</v>
       </c>
-      <c r="H8" s="21">
+      <c r="H8" s="134">
         <v>776.3</v>
       </c>
-      <c r="I8" s="20">
+      <c r="I8" s="135">
         <v>891.7</v>
       </c>
-      <c r="J8" s="19">
+      <c r="J8" s="136">
         <v>873.3</v>
       </c>
-      <c r="K8" s="18">
+      <c r="K8" s="137">
         <f t="shared" si="0"/>
         <v>0.15944540727903012</v>
       </c>
-      <c r="L8" s="17">
+      <c r="L8" s="138">
         <v>0.65</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="21" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:12" ht="20">
       <c r="B9" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="131">
         <v>2967</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="131">
         <v>513</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="132">
         <v>100</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="132">
         <v>100</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="133">
         <v>5</v>
       </c>
-      <c r="H9" s="21">
+      <c r="H9" s="134">
         <v>1011.1</v>
       </c>
-      <c r="I9" s="20">
+      <c r="I9" s="135">
         <v>1165.9000000000001</v>
       </c>
-      <c r="J9" s="19">
+      <c r="J9" s="136">
         <v>1089.9000000000001</v>
       </c>
-      <c r="K9" s="18">
+      <c r="K9" s="137">
         <f t="shared" si="0"/>
         <v>0.49095607235142097</v>
       </c>
-      <c r="L9" s="17">
+      <c r="L9" s="138">
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="21" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:12" ht="20">
       <c r="B10" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="131">
         <v>6466</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="131">
         <v>1728</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="132">
         <v>411</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="132">
         <v>411</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="133">
         <v>6</v>
       </c>
-      <c r="H10" s="21">
+      <c r="H10" s="134">
         <v>822.1</v>
       </c>
-      <c r="I10" s="20">
+      <c r="I10" s="135">
         <v>950.8</v>
       </c>
-      <c r="J10" s="19">
+      <c r="J10" s="136">
         <v>886.6</v>
       </c>
-      <c r="K10" s="18">
+      <c r="K10" s="137">
         <f t="shared" si="0"/>
         <v>0.4988344988344986</v>
       </c>
-      <c r="L10" s="17">
+      <c r="L10" s="138">
         <v>1.33</v>
       </c>
     </row>
-    <row r="11" spans="2:12" ht="21" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:12" ht="20">
       <c r="B11" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="131">
         <v>8422</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="131">
         <v>1564</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="132">
         <v>376</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="132">
         <v>376</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="133">
         <v>6</v>
       </c>
-      <c r="H11" s="21">
+      <c r="H11" s="134">
         <v>798.1</v>
       </c>
-      <c r="I11" s="20">
+      <c r="I11" s="135">
         <v>933.2</v>
       </c>
-      <c r="J11" s="19">
+      <c r="J11" s="136">
         <v>909.8</v>
       </c>
-      <c r="K11" s="18">
+      <c r="K11" s="137">
         <f t="shared" si="0"/>
         <v>0.17320503330866088</v>
       </c>
-      <c r="L11" s="17">
+      <c r="L11" s="138">
         <v>1.46</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="22" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:12" ht="21" thickBot="1">
       <c r="B12" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="139">
         <v>6861</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="139">
         <v>1275</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="140">
         <v>627</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="140">
         <v>557</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="141">
         <v>10</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H12" s="142">
         <v>731.7</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="143">
         <v>842.5</v>
       </c>
-      <c r="J12" s="8">
+      <c r="J12" s="144">
         <v>820.3</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="145">
         <f t="shared" si="0"/>
         <v>0.2003610108303254</v>
       </c>
-      <c r="L12" s="6">
+      <c r="L12" s="146">
         <v>1.43</v>
       </c>
     </row>
-    <row r="13" spans="2:12" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:12" ht="22" thickTop="1" thickBot="1">
       <c r="B13" s="33" t="s">
         <v>2</v>
       </c>
@@ -5036,7 +6741,7 @@
       <c r="J13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K13" s="1">
+      <c r="K13" s="147">
         <f>AVERAGE(K4:K12)</f>
         <v>0.25051152231981499</v>
       </c>
@@ -5044,7 +6749,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="16" thickTop="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="2:12" ht="16" thickTop="1"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="L2:L3"/>
@@ -5064,15 +6769,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:Z14"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
@@ -5094,25 +6799,25 @@
     <col min="25" max="25" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26" ht="16" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:26" ht="22.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="90" t="s">
+    <row r="1" spans="2:26" ht="16" thickBot="1"/>
+    <row r="2" spans="2:26" ht="22.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B2" s="106" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="92" t="s">
+      <c r="D2" s="108" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="87"/>
-      <c r="F2" s="93" t="s">
+      <c r="E2" s="103"/>
+      <c r="F2" s="109" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="93" t="s">
+      <c r="G2" s="109" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="95" t="s">
+      <c r="H2" s="111" t="s">
         <v>27</v>
       </c>
       <c r="K2" s="45" t="s">
@@ -5145,25 +6850,25 @@
       <c r="T2" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="W2" s="97" t="s">
+      <c r="W2" s="113" t="s">
         <v>16</v>
       </c>
-      <c r="X2" s="86" t="s">
+      <c r="X2" s="102" t="s">
         <v>35</v>
       </c>
-      <c r="Y2" s="87"/>
-      <c r="Z2" s="88" t="s">
+      <c r="Y2" s="103"/>
+      <c r="Z2" s="104" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="2:26" ht="22.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="91"/>
+    <row r="3" spans="2:26" ht="22.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B3" s="107"/>
       <c r="C3" s="52"/>
       <c r="D3" s="53"/>
       <c r="E3" s="54"/>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="96"/>
+      <c r="F3" s="110"/>
+      <c r="G3" s="110"/>
+      <c r="H3" s="112"/>
       <c r="K3" s="46" t="s">
         <v>37</v>
       </c>
@@ -5194,16 +6899,16 @@
       <c r="T3" s="22">
         <v>2</v>
       </c>
-      <c r="W3" s="98"/>
+      <c r="W3" s="114"/>
       <c r="X3" s="52" t="s">
         <v>38</v>
       </c>
       <c r="Y3" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="Z3" s="89"/>
+      <c r="Z3" s="105"/>
     </row>
-    <row r="4" spans="2:26" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:26" ht="23" thickTop="1" thickBot="1">
       <c r="B4" s="55" t="s">
         <v>40</v>
       </c>
@@ -5270,7 +6975,7 @@
         <v>34014</v>
       </c>
     </row>
-    <row r="5" spans="2:26" ht="22" thickTop="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:26" ht="22" thickTop="1">
       <c r="B5" s="58" t="s">
         <v>42</v>
       </c>
@@ -5307,7 +7012,7 @@
         <v>4215</v>
       </c>
     </row>
-    <row r="6" spans="2:26" ht="21" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:26" ht="21">
       <c r="B6" s="58" t="s">
         <v>9</v>
       </c>
@@ -5354,7 +7059,7 @@
         <v>7903</v>
       </c>
     </row>
-    <row r="7" spans="2:26" ht="21" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:26" ht="21">
       <c r="B7" s="58" t="s">
         <v>8</v>
       </c>
@@ -5401,7 +7106,7 @@
         <v>30765</v>
       </c>
     </row>
-    <row r="8" spans="2:26" ht="21" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:26" ht="21">
       <c r="B8" s="58" t="s">
         <v>44</v>
       </c>
@@ -5448,7 +7153,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="9" spans="2:26" ht="21" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:26" ht="21">
       <c r="B9" s="58" t="s">
         <v>45</v>
       </c>
@@ -5495,7 +7200,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="2:26" ht="21" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:26" ht="21">
       <c r="B10" s="58" t="s">
         <v>46</v>
       </c>
@@ -5542,7 +7247,7 @@
         <v>2587</v>
       </c>
     </row>
-    <row r="11" spans="2:26" ht="21" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:26" ht="21">
       <c r="B11" s="58" t="s">
         <v>47</v>
       </c>
@@ -5589,7 +7294,7 @@
         <v>3308</v>
       </c>
     </row>
-    <row r="12" spans="2:26" ht="22" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:26" ht="22" thickBot="1">
       <c r="B12" s="61" t="s">
         <v>48</v>
       </c>
@@ -5636,7 +7341,7 @@
         <v>4060</v>
       </c>
     </row>
-    <row r="13" spans="2:26" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:26" ht="23" thickTop="1" thickBot="1">
       <c r="B13" s="64" t="s">
         <v>49</v>
       </c>
@@ -5669,7 +7374,7 @@
       <c r="S13" s="43"/>
       <c r="T13" s="43"/>
     </row>
-    <row r="14" spans="2:26" ht="16" thickTop="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="2:26" ht="16" thickTop="1"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="X2:Y2"/>
@@ -5688,15 +7393,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
@@ -5706,62 +7411,62 @@
     <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:7" ht="22" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="99" t="s">
+    <row r="1" spans="2:7" ht="16" thickBot="1"/>
+    <row r="2" spans="2:7" ht="22" thickTop="1" thickBot="1">
+      <c r="B2" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="100" t="s">
+      <c r="C2" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="101" t="s">
+      <c r="D2" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="101" t="s">
+      <c r="E2" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="101" t="s">
+      <c r="F2" s="74" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="102" t="s">
+      <c r="G2" s="75" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="22" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="103">
+    <row r="3" spans="2:7" ht="22" thickTop="1">
+      <c r="B3" s="76">
         <v>2</v>
       </c>
-      <c r="C3" s="104">
+      <c r="C3" s="77">
         <v>773.9</v>
       </c>
-      <c r="D3" s="105">
+      <c r="D3" s="78">
         <v>897.8</v>
       </c>
-      <c r="E3" s="106">
+      <c r="E3" s="79">
         <v>878.9</v>
       </c>
-      <c r="F3" s="107">
+      <c r="F3" s="80">
         <f>(D3-E3)/(D3-C3)*100%</f>
         <v>0.15254237288135578</v>
       </c>
-      <c r="G3" s="108">
+      <c r="G3" s="81">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="21" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:7" ht="21">
       <c r="B4" s="17">
         <v>3</v>
       </c>
-      <c r="C4" s="109">
+      <c r="C4" s="82">
         <v>773.9</v>
       </c>
-      <c r="D4" s="110">
+      <c r="D4" s="83">
         <v>897.8</v>
       </c>
       <c r="E4" s="15">
         <v>878.9</v>
       </c>
-      <c r="F4" s="111">
+      <c r="F4" s="84">
         <f t="shared" ref="F4:F10" si="0">(D4-E4)/(D4-C4)*100%</f>
         <v>0.15254237288135578</v>
       </c>
@@ -5769,20 +7474,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="21" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:7" ht="21">
       <c r="B5" s="17">
         <v>4</v>
       </c>
-      <c r="C5" s="109">
+      <c r="C5" s="82">
         <v>773.9</v>
       </c>
-      <c r="D5" s="110">
+      <c r="D5" s="83">
         <v>897.8</v>
       </c>
       <c r="E5" s="15">
         <v>875.2</v>
       </c>
-      <c r="F5" s="111">
+      <c r="F5" s="84">
         <f t="shared" si="0"/>
         <v>0.18240516545601221</v>
       </c>
@@ -5790,20 +7495,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="21" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:7" ht="21">
       <c r="B6" s="17">
         <v>5</v>
       </c>
-      <c r="C6" s="109">
+      <c r="C6" s="82">
         <v>773.9</v>
       </c>
-      <c r="D6" s="110">
+      <c r="D6" s="83">
         <v>897.8</v>
       </c>
       <c r="E6" s="15">
         <v>849.9</v>
       </c>
-      <c r="F6" s="111">
+      <c r="F6" s="84">
         <f t="shared" si="0"/>
         <v>0.38660209846650512</v>
       </c>
@@ -5811,20 +7516,20 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="21" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:7" ht="21">
       <c r="B7" s="17">
         <v>6</v>
       </c>
-      <c r="C7" s="109">
+      <c r="C7" s="82">
         <v>773.9</v>
       </c>
-      <c r="D7" s="110">
+      <c r="D7" s="83">
         <v>897.8</v>
       </c>
       <c r="E7" s="15">
         <v>837.2</v>
       </c>
-      <c r="F7" s="111">
+      <c r="F7" s="84">
         <f t="shared" si="0"/>
         <v>0.48910411622275962</v>
       </c>
@@ -5832,20 +7537,20 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="21" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:7" ht="21">
       <c r="B8" s="17">
         <v>7</v>
       </c>
-      <c r="C8" s="109">
+      <c r="C8" s="82">
         <v>773.9</v>
       </c>
-      <c r="D8" s="110">
+      <c r="D8" s="83">
         <v>897.8</v>
       </c>
       <c r="E8" s="15">
         <v>837.2</v>
       </c>
-      <c r="F8" s="111">
+      <c r="F8" s="84">
         <f t="shared" si="0"/>
         <v>0.48910411622275962</v>
       </c>
@@ -5853,20 +7558,20 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="21" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:7" ht="21">
       <c r="B9" s="17">
         <v>8</v>
       </c>
-      <c r="C9" s="109">
+      <c r="C9" s="82">
         <v>773.9</v>
       </c>
-      <c r="D9" s="110">
+      <c r="D9" s="83">
         <v>897.8</v>
       </c>
       <c r="E9" s="15">
         <v>837.2</v>
       </c>
-      <c r="F9" s="111">
+      <c r="F9" s="84">
         <f t="shared" si="0"/>
         <v>0.48910411622275962</v>
       </c>
@@ -5874,20 +7579,20 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="22" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:7" ht="22" thickBot="1">
       <c r="B10" s="6">
         <v>9</v>
       </c>
-      <c r="C10" s="112">
+      <c r="C10" s="85">
         <v>773.9</v>
       </c>
-      <c r="D10" s="113">
+      <c r="D10" s="86">
         <v>897.8</v>
       </c>
       <c r="E10" s="39">
         <v>837.2</v>
       </c>
-      <c r="F10" s="114">
+      <c r="F10" s="87">
         <f t="shared" si="0"/>
         <v>0.48910411622275962</v>
       </c>
@@ -5895,7 +7600,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="16" thickTop="1" x14ac:dyDescent="0.15"/>
+    <row r="11" spans="2:7" ht="16" thickTop="1"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
18/4/12 Write correlation btw Vth and BTI (full done)
</commit_message>
<xml_diff>
--- a/DATE2018/exp/maui_exp.xlsx
+++ b/DATE2018/exp/maui_exp.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erictseng 1/Desktop/LaTeX/MAUI-Latex/DATE2018/exp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/TienHungTseng/Desktop/LaTex/MAUI-LaTeX/DATE2018/exp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{23FCC190-0E67-214D-935C-E8E82B390267}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{D4C22032-D6FA-934C-B4F6-56F34E1AC20D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8320" yWindow="2200" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Benchmark info (2)" sheetId="7" r:id="rId1"/>
@@ -1244,48 +1244,147 @@
     <xf numFmtId="10" fontId="6" fillId="0" borderId="7" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1324,105 +1423,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2782,8 +2782,8 @@
       <xdr:rowOff>202138</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="753155" cy="266355"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="文字方塊 1">
@@ -2910,7 +2910,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="文字方塊 1">
@@ -3049,8 +3049,8 @@
       <xdr:rowOff>219072</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="706604" cy="266611"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="文字方塊 2">
@@ -3177,7 +3177,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="文字方塊 2">
@@ -3316,8 +3316,8 @@
       <xdr:rowOff>203198</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1015343" cy="266611"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="文字方塊 3">
@@ -3468,7 +3468,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="文字方塊 3">
@@ -3607,8 +3607,8 @@
       <xdr:rowOff>203198</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1015343" cy="266611"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="文字方塊 4">
@@ -3759,7 +3759,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="文字方塊 4">
@@ -3903,8 +3903,8 @@
       <xdr:rowOff>202138</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="753155" cy="266355"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="文字方塊 1">
@@ -4033,7 +4033,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="文字方塊 1">
@@ -5863,66 +5863,66 @@
   <sheetData>
     <row r="1" spans="2:13" ht="16" thickBot="1"/>
     <row r="2" spans="2:13" ht="22.75" customHeight="1" thickTop="1">
-      <c r="B2" s="92" t="s">
+      <c r="B2" s="123" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="90" t="s">
+      <c r="C2" s="126" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="90" t="s">
+      <c r="D2" s="126" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="94" t="s">
+      <c r="E2" s="129" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="94" t="s">
+      <c r="F2" s="129" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="96" t="s">
+      <c r="G2" s="132" t="s">
         <v>12</v>
       </c>
       <c r="H2" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="98" t="s">
+      <c r="I2" s="116" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="99"/>
-      <c r="K2" s="99"/>
-      <c r="L2" s="100" t="s">
+      <c r="J2" s="117"/>
+      <c r="K2" s="117"/>
+      <c r="L2" s="118" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="88" t="s">
+      <c r="M2" s="121" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="2:13" ht="22.75" customHeight="1">
-      <c r="B3" s="115"/>
-      <c r="C3" s="116"/>
-      <c r="D3" s="116"/>
-      <c r="E3" s="117"/>
-      <c r="F3" s="117"/>
-      <c r="G3" s="118"/>
-      <c r="H3" s="119"/>
-      <c r="I3" s="120"/>
-      <c r="J3" s="121"/>
-      <c r="K3" s="121"/>
-      <c r="L3" s="122"/>
-      <c r="M3" s="122"/>
+      <c r="B3" s="124"/>
+      <c r="C3" s="127"/>
+      <c r="D3" s="127"/>
+      <c r="E3" s="130"/>
+      <c r="F3" s="130"/>
+      <c r="G3" s="133"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="119"/>
+      <c r="M3" s="119"/>
     </row>
     <row r="4" spans="2:13" ht="56" customHeight="1" thickBot="1">
-      <c r="B4" s="93"/>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="95"/>
-      <c r="F4" s="95"/>
-      <c r="G4" s="97"/>
+      <c r="B4" s="125"/>
+      <c r="C4" s="128"/>
+      <c r="D4" s="128"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="131"/>
+      <c r="G4" s="134"/>
       <c r="H4" s="35"/>
       <c r="I4" s="36"/>
       <c r="J4" s="37"/>
       <c r="K4" s="37"/>
-      <c r="L4" s="101"/>
-      <c r="M4" s="89"/>
+      <c r="L4" s="120"/>
+      <c r="M4" s="122"/>
     </row>
     <row r="5" spans="2:13" ht="22" thickTop="1">
       <c r="B5" s="30" t="s">
@@ -6326,10 +6326,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:L14"/>
+  <dimension ref="B1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6352,378 +6352,390 @@
     <col min="19" max="19" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="16" thickBot="1"/>
-    <row r="2" spans="2:12" ht="22.75" customHeight="1" thickTop="1">
-      <c r="B2" s="92" t="s">
+    <row r="1" spans="2:14" ht="16" thickBot="1"/>
+    <row r="2" spans="2:14" ht="22.75" customHeight="1" thickTop="1">
+      <c r="B2" s="123" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="90" t="s">
+      <c r="C2" s="126" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="90" t="s">
+      <c r="D2" s="126" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="94" t="s">
+      <c r="E2" s="129" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="94" t="s">
+      <c r="F2" s="129" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="96" t="s">
+      <c r="G2" s="132" t="s">
         <v>12</v>
       </c>
       <c r="H2" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="98" t="s">
+      <c r="I2" s="116" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="99"/>
-      <c r="K2" s="100" t="s">
+      <c r="J2" s="117"/>
+      <c r="K2" s="118" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="88" t="s">
+      <c r="L2" s="121" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="56" customHeight="1" thickBot="1">
-      <c r="B3" s="93"/>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="97"/>
+    <row r="3" spans="2:14" ht="56" customHeight="1" thickBot="1">
+      <c r="B3" s="125"/>
+      <c r="C3" s="128"/>
+      <c r="D3" s="128"/>
+      <c r="E3" s="131"/>
+      <c r="F3" s="131"/>
+      <c r="G3" s="134"/>
       <c r="H3" s="35"/>
       <c r="I3" s="36"/>
       <c r="J3" s="37"/>
-      <c r="K3" s="101"/>
-      <c r="L3" s="89"/>
+      <c r="K3" s="120"/>
+      <c r="L3" s="122"/>
     </row>
-    <row r="4" spans="2:12" ht="21" thickTop="1">
+    <row r="4" spans="2:14" ht="21" thickTop="1">
       <c r="B4" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="123">
+      <c r="C4" s="91">
         <v>7401</v>
       </c>
-      <c r="D4" s="123">
+      <c r="D4" s="91">
         <v>8802</v>
       </c>
-      <c r="E4" s="124">
+      <c r="E4" s="92">
         <v>3416</v>
       </c>
-      <c r="F4" s="124">
+      <c r="F4" s="92">
         <v>3416</v>
       </c>
-      <c r="G4" s="125">
+      <c r="G4" s="93">
         <v>11</v>
       </c>
-      <c r="H4" s="126">
+      <c r="H4" s="94">
         <v>773.9</v>
       </c>
-      <c r="I4" s="127">
+      <c r="I4" s="95">
         <v>897.8</v>
       </c>
-      <c r="J4" s="128">
+      <c r="J4" s="96">
         <v>849.9</v>
       </c>
-      <c r="K4" s="129">
+      <c r="K4" s="97">
         <f t="shared" ref="K4:K12" si="0">(I4-J4)/(I4-H4)*100%</f>
         <v>0.38660209846650512</v>
       </c>
-      <c r="L4" s="130">
-        <v>16.45</v>
+      <c r="L4" s="98">
+        <v>18.38</v>
+      </c>
+      <c r="N4">
+        <v>33.700000000000003</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="20">
+    <row r="5" spans="2:14" ht="20">
       <c r="B5" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="131">
+      <c r="C5" s="99">
         <v>526297</v>
       </c>
-      <c r="D5" s="131">
+      <c r="D5" s="99">
         <v>108839</v>
       </c>
-      <c r="E5" s="132">
+      <c r="E5" s="100">
         <v>26863</v>
       </c>
-      <c r="F5" s="132">
+      <c r="F5" s="100">
         <v>4924</v>
       </c>
-      <c r="G5" s="133">
+      <c r="G5" s="101">
         <v>10</v>
       </c>
-      <c r="H5" s="134">
+      <c r="H5" s="102">
         <v>3016.7</v>
       </c>
-      <c r="I5" s="135">
+      <c r="I5" s="103">
         <v>3530.6</v>
       </c>
-      <c r="J5" s="136">
+      <c r="J5" s="104">
         <v>3458.5</v>
       </c>
-      <c r="K5" s="137">
+      <c r="K5" s="105">
         <f t="shared" si="0"/>
         <v>0.14029966919634149</v>
       </c>
-      <c r="L5" s="138">
+      <c r="L5" s="106">
         <v>24.89</v>
       </c>
+      <c r="N5">
+        <v>56</v>
+      </c>
     </row>
-    <row r="6" spans="2:12" ht="20">
+    <row r="6" spans="2:14" ht="20">
       <c r="B6" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="131">
+      <c r="C6" s="99">
         <v>561091</v>
       </c>
-      <c r="D6" s="131">
+      <c r="D6" s="99">
         <v>97831</v>
       </c>
-      <c r="E6" s="132">
+      <c r="E6" s="100">
         <v>33651</v>
       </c>
-      <c r="F6" s="132">
+      <c r="F6" s="100">
         <v>7904</v>
       </c>
-      <c r="G6" s="133">
+      <c r="G6" s="101">
         <v>12</v>
       </c>
-      <c r="H6" s="134">
+      <c r="H6" s="102">
         <v>3367</v>
       </c>
-      <c r="I6" s="135">
+      <c r="I6" s="103">
         <v>3940.2</v>
       </c>
-      <c r="J6" s="136">
+      <c r="J6" s="104">
         <v>3897.9</v>
       </c>
-      <c r="K6" s="137">
+      <c r="K6" s="105">
         <f t="shared" si="0"/>
         <v>7.3796231681786006E-2</v>
       </c>
-      <c r="L6" s="138">
+      <c r="L6" s="106">
         <v>30.69</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="20">
+    <row r="7" spans="2:14" ht="20">
       <c r="B7" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="131">
+      <c r="C7" s="99">
         <v>101496</v>
       </c>
-      <c r="D7" s="131">
+      <c r="D7" s="99">
         <v>17079</v>
       </c>
-      <c r="E7" s="132">
+      <c r="E7" s="100">
         <v>5030</v>
       </c>
-      <c r="F7" s="132">
+      <c r="F7" s="100">
         <v>4345</v>
       </c>
-      <c r="G7" s="133">
+      <c r="G7" s="101">
         <v>10</v>
       </c>
-      <c r="H7" s="134">
+      <c r="H7" s="102">
         <v>864.2</v>
       </c>
-      <c r="I7" s="135">
+      <c r="I7" s="103">
         <v>1013.7</v>
       </c>
-      <c r="J7" s="136">
+      <c r="J7" s="104">
         <v>994.1</v>
       </c>
-      <c r="K7" s="137">
+      <c r="K7" s="105">
         <f t="shared" si="0"/>
         <v>0.13110367892976604</v>
       </c>
-      <c r="L7" s="138">
+      <c r="L7" s="106">
         <v>32.770000000000003</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="20">
+    <row r="8" spans="2:14" ht="20">
       <c r="B8" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="131">
+      <c r="C8" s="99">
         <v>2627</v>
       </c>
-      <c r="D8" s="131">
+      <c r="D8" s="99">
         <v>625</v>
       </c>
-      <c r="E8" s="132">
+      <c r="E8" s="100">
         <v>186</v>
       </c>
-      <c r="F8" s="132">
+      <c r="F8" s="100">
         <v>180</v>
       </c>
-      <c r="G8" s="133">
+      <c r="G8" s="101">
         <v>8</v>
       </c>
-      <c r="H8" s="134">
+      <c r="H8" s="102">
         <v>776.3</v>
       </c>
-      <c r="I8" s="135">
+      <c r="I8" s="103">
         <v>891.7</v>
       </c>
-      <c r="J8" s="136">
+      <c r="J8" s="104">
         <v>873.3</v>
       </c>
-      <c r="K8" s="137">
+      <c r="K8" s="105">
         <f t="shared" si="0"/>
         <v>0.15944540727903012</v>
       </c>
-      <c r="L8" s="138">
+      <c r="L8" s="106">
         <v>0.65</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="20">
+    <row r="9" spans="2:14" ht="20">
       <c r="B9" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="131">
+      <c r="C9" s="99">
         <v>2967</v>
       </c>
-      <c r="D9" s="131">
+      <c r="D9" s="99">
         <v>513</v>
       </c>
-      <c r="E9" s="132">
+      <c r="E9" s="100">
         <v>100</v>
       </c>
-      <c r="F9" s="132">
+      <c r="F9" s="100">
         <v>100</v>
       </c>
-      <c r="G9" s="133">
+      <c r="G9" s="101">
         <v>5</v>
       </c>
-      <c r="H9" s="134">
+      <c r="H9" s="102">
         <v>1011.1</v>
       </c>
-      <c r="I9" s="135">
+      <c r="I9" s="103">
         <v>1165.9000000000001</v>
       </c>
-      <c r="J9" s="136">
+      <c r="J9" s="104">
         <v>1089.9000000000001</v>
       </c>
-      <c r="K9" s="137">
+      <c r="K9" s="105">
         <f t="shared" si="0"/>
         <v>0.49095607235142097</v>
       </c>
-      <c r="L9" s="138">
+      <c r="L9" s="106">
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="20">
+    <row r="10" spans="2:14" ht="20">
       <c r="B10" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="131">
+      <c r="C10" s="99">
         <v>6466</v>
       </c>
-      <c r="D10" s="131">
+      <c r="D10" s="99">
         <v>1728</v>
       </c>
-      <c r="E10" s="132">
+      <c r="E10" s="100">
         <v>411</v>
       </c>
-      <c r="F10" s="132">
+      <c r="F10" s="100">
         <v>411</v>
       </c>
-      <c r="G10" s="133">
+      <c r="G10" s="101">
         <v>6</v>
       </c>
-      <c r="H10" s="134">
+      <c r="H10" s="102">
         <v>822.1</v>
       </c>
-      <c r="I10" s="135">
+      <c r="I10" s="103">
         <v>950.8</v>
       </c>
-      <c r="J10" s="136">
+      <c r="J10" s="104">
         <v>886.6</v>
       </c>
-      <c r="K10" s="137">
+      <c r="K10" s="105">
         <f t="shared" si="0"/>
         <v>0.4988344988344986</v>
       </c>
-      <c r="L10" s="138">
+      <c r="L10" s="106">
         <v>1.33</v>
       </c>
     </row>
-    <row r="11" spans="2:12" ht="20">
+    <row r="11" spans="2:14" ht="20">
       <c r="B11" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="131">
+      <c r="C11" s="99">
         <v>8422</v>
       </c>
-      <c r="D11" s="131">
+      <c r="D11" s="99">
         <v>1564</v>
       </c>
-      <c r="E11" s="132">
+      <c r="E11" s="100">
         <v>376</v>
       </c>
-      <c r="F11" s="132">
+      <c r="F11" s="100">
         <v>376</v>
       </c>
-      <c r="G11" s="133">
+      <c r="G11" s="101">
         <v>6</v>
       </c>
-      <c r="H11" s="134">
+      <c r="H11" s="102">
         <v>798.1</v>
       </c>
-      <c r="I11" s="135">
+      <c r="I11" s="103">
         <v>933.2</v>
       </c>
-      <c r="J11" s="136">
+      <c r="J11" s="104">
         <v>909.8</v>
       </c>
-      <c r="K11" s="137">
+      <c r="K11" s="105">
         <f t="shared" si="0"/>
         <v>0.17320503330866088</v>
       </c>
-      <c r="L11" s="138">
+      <c r="L11" s="106">
         <v>1.46</v>
       </c>
+      <c r="N11">
+        <v>3.0819999999999999</v>
+      </c>
     </row>
-    <row r="12" spans="2:12" ht="21" thickBot="1">
+    <row r="12" spans="2:14" ht="21" thickBot="1">
       <c r="B12" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="139">
+      <c r="C12" s="107">
         <v>6861</v>
       </c>
-      <c r="D12" s="139">
+      <c r="D12" s="107">
         <v>1275</v>
       </c>
-      <c r="E12" s="140">
+      <c r="E12" s="108">
         <v>627</v>
       </c>
-      <c r="F12" s="140">
+      <c r="F12" s="108">
         <v>557</v>
       </c>
-      <c r="G12" s="141">
+      <c r="G12" s="109">
         <v>10</v>
       </c>
-      <c r="H12" s="142">
+      <c r="H12" s="110">
         <v>731.7</v>
       </c>
-      <c r="I12" s="143">
+      <c r="I12" s="111">
         <v>842.5</v>
       </c>
-      <c r="J12" s="144">
+      <c r="J12" s="112">
         <v>820.3</v>
       </c>
-      <c r="K12" s="145">
+      <c r="K12" s="113">
         <f t="shared" si="0"/>
         <v>0.2003610108303254</v>
       </c>
-      <c r="L12" s="146">
+      <c r="L12" s="114">
         <v>1.43</v>
       </c>
+      <c r="N12">
+        <v>3.5501299999999998</v>
+      </c>
     </row>
-    <row r="13" spans="2:12" ht="22" thickTop="1" thickBot="1">
+    <row r="13" spans="2:14" ht="22" thickTop="1" thickBot="1">
       <c r="B13" s="33" t="s">
         <v>2</v>
       </c>
@@ -6741,7 +6753,7 @@
       <c r="J13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K13" s="147">
+      <c r="K13" s="115">
         <f>AVERAGE(K4:K12)</f>
         <v>0.25051152231981499</v>
       </c>
@@ -6749,7 +6761,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="16" thickTop="1"/>
+    <row r="14" spans="2:14" ht="16" thickTop="1"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="L2:L3"/>
@@ -6801,23 +6813,23 @@
   <sheetData>
     <row r="1" spans="2:26" ht="16" thickBot="1"/>
     <row r="2" spans="2:26" ht="22.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="106" t="s">
+      <c r="B2" s="139" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="108" t="s">
+      <c r="D2" s="141" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="103"/>
-      <c r="F2" s="109" t="s">
+      <c r="E2" s="136"/>
+      <c r="F2" s="142" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="109" t="s">
+      <c r="G2" s="142" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="111" t="s">
+      <c r="H2" s="144" t="s">
         <v>27</v>
       </c>
       <c r="K2" s="45" t="s">
@@ -6850,25 +6862,25 @@
       <c r="T2" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="W2" s="113" t="s">
+      <c r="W2" s="146" t="s">
         <v>16</v>
       </c>
-      <c r="X2" s="102" t="s">
+      <c r="X2" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="Y2" s="103"/>
-      <c r="Z2" s="104" t="s">
+      <c r="Y2" s="136"/>
+      <c r="Z2" s="137" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="3" spans="2:26" ht="22.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B3" s="107"/>
+      <c r="B3" s="140"/>
       <c r="C3" s="52"/>
       <c r="D3" s="53"/>
       <c r="E3" s="54"/>
-      <c r="F3" s="110"/>
-      <c r="G3" s="110"/>
-      <c r="H3" s="112"/>
+      <c r="F3" s="143"/>
+      <c r="G3" s="143"/>
+      <c r="H3" s="145"/>
       <c r="K3" s="46" t="s">
         <v>37</v>
       </c>
@@ -6899,14 +6911,14 @@
       <c r="T3" s="22">
         <v>2</v>
       </c>
-      <c r="W3" s="114"/>
+      <c r="W3" s="147"/>
       <c r="X3" s="52" t="s">
         <v>38</v>
       </c>
       <c r="Y3" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="Z3" s="105"/>
+      <c r="Z3" s="138"/>
     </row>
     <row r="4" spans="2:26" ht="23" thickTop="1" thickBot="1">
       <c r="B4" s="55" t="s">

</xml_diff>